<commit_message>
excel.py was also changed to polars from pandas.
</commit_message>
<xml_diff>
--- a/testdata/one.xlsx
+++ b/testdata/one.xlsx
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>province</t>
-  </si>
-  <si>
-    <t>tazkira</t>
-  </si>
-  <si>
-    <t>farhad</t>
-  </si>
-  <si>
-    <t>kabul</t>
+    <t>country</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Iran</t>
   </si>
 </sst>
 </file>
@@ -289,19 +289,29 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2025.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1">
+        <v>2025.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>100045.0</v>
+      <c r="B4" s="1">
+        <v>2025.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>